<commit_message>
Replaced OPA221 w/ OPA188
</commit_message>
<xml_diff>
--- a/Forms/Build_Order.xlsx
+++ b/Forms/Build_Order.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="111">
   <si>
     <t>Name</t>
   </si>
@@ -125,12 +125,6 @@
     <t>http://www.mouser.com/ProductDetail/Texas-Instruments/INA128UA</t>
   </si>
   <si>
-    <t>OPA2228UA</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/Texas-Instruments/OPA2228UA</t>
-  </si>
-  <si>
     <t>1N4148W-E3-08</t>
   </si>
   <si>
@@ -221,9 +215,6 @@
     <t>2.2 µH Inductor</t>
   </si>
   <si>
-    <t>2x1.5x1mm</t>
-  </si>
-  <si>
     <t>http://www.mouser.com/ProductDetail/TDK/TFM201610ALM-2R2MTAA</t>
   </si>
   <si>
@@ -326,22 +317,49 @@
     <t>http://www.mouser.com/ProductDetail/Vishay-Dale/CRCW120651R0FKEA</t>
   </si>
   <si>
-    <t>http://www.mouser.com/ProductDetail/TDK/CGA3E2C0G1H103J080AA</t>
-  </si>
-  <si>
-    <t>0.01 µF NP Capacitor</t>
-  </si>
-  <si>
-    <t>CGA3E2C0G1H103J080AA</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/Vishay-Dale/CRCW120651K0FKEA</t>
-  </si>
-  <si>
-    <t>51 kΩ Resistor</t>
-  </si>
-  <si>
-    <t>CRCW120651K0FKEA</t>
+    <t>CRCW12065M10FKEA</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay-Dale/CRCW12065M10FKEA</t>
+  </si>
+  <si>
+    <t>5.1 MΩ Resistor</t>
+  </si>
+  <si>
+    <t>75 kΩ Resistor</t>
+  </si>
+  <si>
+    <t>CRCW120675K0FKEA</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay-Dale/CRCW120675K0FKEA</t>
+  </si>
+  <si>
+    <t>CRCW12067K50FKEA</t>
+  </si>
+  <si>
+    <t>7.5 kΩ Resistor</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay-Dale/CRCW12067K50FKEA</t>
+  </si>
+  <si>
+    <t>L2016</t>
+  </si>
+  <si>
+    <t>CRCW12065M00FKEA</t>
+  </si>
+  <si>
+    <t>1 MΩ Resistor</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay-Dale/CRCW12061M00FKEA</t>
+  </si>
+  <si>
+    <t>OPA2188AIDR</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Texas-Instruments/OPA2188AIDR</t>
   </si>
 </sst>
 </file>
@@ -427,7 +445,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -464,9 +482,6 @@
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -882,10 +897,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="95" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="95" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -940,14 +955,14 @@
       </c>
       <c r="B3" s="18">
         <f ca="1">TODAY()</f>
-        <v>42646</v>
-      </c>
-      <c r="C3" s="21" t="s">
+        <v>42648</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1017,23 +1032,23 @@
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F7" s="13">
         <v>1.93</v>
       </c>
       <c r="G7" s="13">
-        <f t="shared" ref="G7:G11" si="0">B7*F7</f>
+        <f t="shared" ref="G7:G10" si="0">B7*F7</f>
         <v>3.86</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1062,7 +1077,7 @@
       <c r="H8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="20"/>
+      <c r="I8" s="19"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
@@ -1072,7 +1087,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>26</v>
@@ -1081,16 +1096,16 @@
         <v>29</v>
       </c>
       <c r="F9" s="13">
-        <v>5.53</v>
+        <v>3.33</v>
       </c>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
-        <v>38.71</v>
+        <v>23.310000000000002</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="20"/>
+        <v>110</v>
+      </c>
+      <c r="I9" s="19"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
@@ -1100,13 +1115,13 @@
         <v>2</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F10" s="13">
         <v>0.1</v>
@@ -1116,63 +1131,62 @@
         <v>0.2</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="6">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>101</v>
+        <v>47</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="E11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="G11" s="13">
+        <f t="shared" ref="G11:G31" si="1">B11*F11</f>
+        <v>5</v>
+      </c>
+      <c r="H11" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="13">
-        <v>0.34</v>
-      </c>
-      <c r="G11" s="13">
-        <f t="shared" si="0"/>
-        <v>2.72</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="I11" s="19"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="6">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F12" s="13">
-        <v>0.2</v>
+        <v>0.26</v>
       </c>
       <c r="G12" s="13">
-        <f t="shared" ref="G12:G29" si="1">B12*F12</f>
-        <v>4.2</v>
+        <f>B12*F12</f>
+        <v>0.78</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1183,23 +1197,23 @@
         <v>3</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="F13" s="13">
-        <v>0.26</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="G13" s="13">
-        <f>B13*F13</f>
-        <v>0.78</v>
+        <f t="shared" si="1"/>
+        <v>1.6800000000000002</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1207,26 +1221,26 @@
         <v>24</v>
       </c>
       <c r="B14" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F14" s="13">
-        <v>0.56000000000000005</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="G14" s="13">
         <f t="shared" si="1"/>
-        <v>1.6800000000000002</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1234,26 +1248,26 @@
         <v>24</v>
       </c>
       <c r="B15" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="F15" s="13">
-        <v>1.1100000000000001</v>
+        <v>0.39</v>
       </c>
       <c r="G15" s="13">
         <f t="shared" si="1"/>
-        <v>2.2200000000000002</v>
+        <v>0.39</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1261,26 +1275,26 @@
         <v>24</v>
       </c>
       <c r="B16" s="6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F16" s="13">
-        <v>0.39</v>
+        <v>0.23</v>
       </c>
       <c r="G16" s="13">
         <f t="shared" si="1"/>
-        <v>0.39</v>
+        <v>1.3800000000000001</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1288,26 +1302,26 @@
         <v>24</v>
       </c>
       <c r="B17" s="6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="F17" s="13">
-        <v>0.23</v>
+        <v>0.1</v>
       </c>
       <c r="G17" s="13">
         <f t="shared" si="1"/>
-        <v>1.3800000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1315,26 +1329,26 @@
         <v>24</v>
       </c>
       <c r="B18" s="6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F18" s="13">
         <v>0.1</v>
       </c>
       <c r="G18" s="13">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1342,26 +1356,26 @@
         <v>24</v>
       </c>
       <c r="B19" s="6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>90</v>
+        <v>41</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>45</v>
       </c>
       <c r="F19" s="13">
         <v>0.1</v>
       </c>
       <c r="G19" s="13">
-        <f t="shared" si="1"/>
-        <v>0.60000000000000009</v>
+        <f>B19*F19</f>
+        <v>0.4</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1372,13 +1386,13 @@
         <v>4</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>43</v>
+        <v>102</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F20" s="13">
         <v>0.1</v>
@@ -1388,7 +1402,7 @@
         <v>0.4</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1396,26 +1410,26 @@
         <v>24</v>
       </c>
       <c r="B21" s="6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F21" s="13">
         <v>0.1</v>
       </c>
       <c r="G21" s="13">
         <f>B21*F21</f>
-        <v>0.60000000000000009</v>
+        <v>0.2</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1426,13 +1440,13 @@
         <v>4</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F22" s="13">
         <v>0.1</v>
@@ -1442,7 +1456,7 @@
         <v>0.4</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1450,26 +1464,26 @@
         <v>24</v>
       </c>
       <c r="B23" s="6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F23" s="13">
         <v>0.1</v>
       </c>
       <c r="G23" s="13">
         <f t="shared" si="1"/>
-        <v>0.60000000000000009</v>
+        <v>0.4</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1480,13 +1494,13 @@
         <v>1</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F24" s="13">
         <v>0.1</v>
@@ -1496,7 +1510,7 @@
         <v>0.1</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1504,26 +1518,26 @@
         <v>24</v>
       </c>
       <c r="B25" s="6">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F25" s="13">
         <v>0.11</v>
       </c>
       <c r="G25" s="13">
         <f t="shared" si="1"/>
-        <v>0.88</v>
+        <v>0.22</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1534,13 +1548,13 @@
         <v>1</v>
       </c>
       <c r="C26" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="E26" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F26" s="13">
         <v>0.1</v>
@@ -1550,7 +1564,7 @@
         <v>0.1</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1561,23 +1575,23 @@
         <v>2</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="F27" s="13">
-        <v>0.69</v>
+        <v>0.1</v>
       </c>
       <c r="G27" s="13">
         <f t="shared" si="1"/>
-        <v>1.38</v>
+        <v>0.2</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1585,26 +1599,26 @@
         <v>24</v>
       </c>
       <c r="B28" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>57</v>
+        <v>98</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>45</v>
       </c>
       <c r="F28" s="13">
-        <v>3.59</v>
+        <v>0.1</v>
       </c>
       <c r="G28" s="13">
         <f t="shared" si="1"/>
-        <v>3.59</v>
+        <v>0.2</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1612,32 +1626,86 @@
         <v>24</v>
       </c>
       <c r="B29" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>88</v>
+        <v>61</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>105</v>
       </c>
       <c r="F29" s="13">
-        <v>0.75</v>
+        <v>0.69</v>
       </c>
       <c r="G29" s="13">
         <f t="shared" si="1"/>
+        <v>1.38</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="6">
+        <v>1</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" s="13">
+        <v>3.59</v>
+      </c>
+      <c r="G30" s="13">
+        <f t="shared" si="1"/>
+        <v>3.59</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="6">
+        <v>1</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="13">
         <v>0.75</v>
       </c>
-      <c r="H29" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G37" s="13">
-        <f>SUM(G7:G29)</f>
-        <v>82.47999999999999</v>
+      <c r="G31" s="13">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G39" s="13">
+        <f>SUM(G7:G31)</f>
+        <v>64.700000000000017</v>
       </c>
     </row>
   </sheetData>
@@ -1650,27 +1718,29 @@
     <hyperlink ref="H9" r:id="rId1"/>
     <hyperlink ref="H8" r:id="rId2"/>
     <hyperlink ref="H7" r:id="rId3"/>
-    <hyperlink ref="H14" r:id="rId4"/>
-    <hyperlink ref="H17" r:id="rId5"/>
+    <hyperlink ref="H13" r:id="rId4"/>
+    <hyperlink ref="H16" r:id="rId5"/>
     <hyperlink ref="H21" r:id="rId6"/>
     <hyperlink ref="H25" r:id="rId7"/>
-    <hyperlink ref="H20" r:id="rId8"/>
-    <hyperlink ref="H13" r:id="rId9"/>
-    <hyperlink ref="H28" r:id="rId10"/>
-    <hyperlink ref="H15" r:id="rId11"/>
+    <hyperlink ref="H19" r:id="rId8"/>
+    <hyperlink ref="H12" r:id="rId9"/>
+    <hyperlink ref="H30" r:id="rId10"/>
+    <hyperlink ref="H14" r:id="rId11"/>
     <hyperlink ref="H23" r:id="rId12"/>
     <hyperlink ref="H24" r:id="rId13"/>
     <hyperlink ref="H26" r:id="rId14"/>
-    <hyperlink ref="H16" r:id="rId15"/>
-    <hyperlink ref="H27" r:id="rId16"/>
-    <hyperlink ref="H29" r:id="rId17"/>
-    <hyperlink ref="H19" r:id="rId18"/>
+    <hyperlink ref="H15" r:id="rId15"/>
+    <hyperlink ref="H29" r:id="rId16"/>
+    <hyperlink ref="H31" r:id="rId17"/>
+    <hyperlink ref="H18" r:id="rId18"/>
     <hyperlink ref="H10" r:id="rId19"/>
-    <hyperlink ref="H18" r:id="rId20"/>
-    <hyperlink ref="H11" r:id="rId21"/>
-    <hyperlink ref="H22" r:id="rId22"/>
+    <hyperlink ref="H17" r:id="rId20"/>
+    <hyperlink ref="H22" r:id="rId21"/>
+    <hyperlink ref="H28" r:id="rId22"/>
+    <hyperlink ref="H20" r:id="rId23"/>
+    <hyperlink ref="H27" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId23"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>